<commit_message>
feat(menu): Add quit button
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">CRÉDITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN_QUIT_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUITTER</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -306,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -406,6 +415,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(menu): Ask for confirmation before quitting
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -71,6 +71,33 @@
   </si>
   <si>
     <t xml:space="preserve">QUITTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIT_CONFIRM_TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are quitting the game, are you sure?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tu vas quitter le jeu, tu es sûr ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIT_CONFIRM_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIT_CONFIRM_CANCEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuter</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -315,10 +342,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,6 +453,39 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(console): create UI for GameConsole
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -97,7 +97,25 @@
     <t xml:space="preserve">Cancel</t>
   </si>
   <si>
-    <t xml:space="preserve">Annuter</t>
+    <t xml:space="preserve">Annuler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSOLE_INPUT_PLACEHOLDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter command here…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entre une commande ici…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSOLE_INPUT_SUBMIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoyer</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -342,15 +360,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
   </cols>
   <sheetData>
@@ -484,6 +502,28 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix old Godot versio shown
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">GAME_NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">Godot 4.2</t>
+    <t xml:space="preserve">Godot 4.3</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_TAGLINE</t>
@@ -363,7 +363,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat(console): implement a game console (#2)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">GAME_NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">Godot 4.2</t>
+    <t xml:space="preserve">Godot 4.3</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_TAGLINE</t>
@@ -97,7 +97,25 @@
     <t xml:space="preserve">Cancel</t>
   </si>
   <si>
-    <t xml:space="preserve">Annuter</t>
+    <t xml:space="preserve">Annuler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSOLE_INPUT_PLACEHOLDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter command here…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entre une commande ici…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSOLE_INPUT_SUBMIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoyer</t>
   </si>
   <si>
     <t xml:space="preserve">CREDITS_TAGLINE</t>
@@ -342,15 +360,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
   </cols>
   <sheetData>
@@ -484,6 +502,28 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>